<commit_message>
revisi terbari hanya akurasi
</commit_message>
<xml_diff>
--- a/datasetCovid.xlsx
+++ b/datasetCovid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMI FARIZKI\UNSRI\MK\SKRIPSI\SVM\SKRIPSI\PROGRAM\python\flaskSkripsiFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMI FARIZKI\UNSRI\MK\SKRIPSI\SVM\SKRIPSI\PROGRAM\python\SVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AE7E88-E2DA-4030-BD41-B0F87A1F1E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A8C5E9-57CD-462F-A387-4697AAB02EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B289C505-5B93-4543-A7A9-FF99ABFE1CBF}"/>
   </bookViews>
@@ -3390,8 +3390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA23EBFA-A1EF-46D8-A54B-2ED224BC79DC}">
   <dimension ref="A1:C831"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8620,7 +8620,7 @@
         <v>474</v>
       </c>
       <c r="B475" t="s">
-        <v>0</v>
+        <v>474</v>
       </c>
       <c r="C475" s="2" t="s">
         <v>428</v>

</xml_diff>

<commit_message>
push terbaru cv tidak interface
</commit_message>
<xml_diff>
--- a/datasetCovid.xlsx
+++ b/datasetCovid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMI FARIZKI\UNSRI\MK\SKRIPSI\SVM\SKRIPSI\PROGRAM\python\FINALSKRIPSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMI FARIZKI\UNSRI\MK\SKRIPSI\SVM\SKRIPSI\PROGRAM\python\FINALSKRIPSI - REVISI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBC743C-082B-41B6-829D-4C70C6EA46F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C077226-2D7B-4B72-AD7C-FE4DF157522E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B289C505-5B93-4543-A7A9-FF99ABFE1CBF}"/>
   </bookViews>
@@ -2667,7 +2667,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3410,7 +3430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3420,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA23EBFA-A1EF-46D8-A54B-2ED224BC79DC}">
   <dimension ref="A1:C831"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A700" workbookViewId="0">
+      <selection activeCell="C701" sqref="C701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8524,59 +8544,59 @@
         <v>416</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A464">
         <v>463</v>
       </c>
       <c r="B464" t="s">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="C464" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="465" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A465">
         <v>464</v>
       </c>
       <c r="B465" t="s">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="C465" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="466" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A466">
         <v>465</v>
       </c>
       <c r="B466" t="s">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="467" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A467">
         <v>466</v>
       </c>
       <c r="B467" t="s">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="C467" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="468" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A468">
         <v>467</v>
       </c>
       <c r="B468" t="s">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>421</v>
+        <v>634</v>
       </c>
     </row>
     <row r="469" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -11087,59 +11107,59 @@
         <v>630</v>
       </c>
     </row>
-    <row r="697" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="697" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A697">
         <v>696</v>
       </c>
       <c r="B697" t="s">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="698" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="698" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A698">
         <v>697</v>
       </c>
       <c r="B698" t="s">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="699" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="699" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A699">
         <v>698</v>
       </c>
       <c r="B699" t="s">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="700" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="700" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A700">
         <v>699</v>
       </c>
       <c r="B700" t="s">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="701" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="701" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A701">
         <v>700</v>
       </c>
       <c r="B701" t="s">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="C701" s="2" t="s">
-        <v>634</v>
+        <v>421</v>
       </c>
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.35">
@@ -11527,136 +11547,142 @@
       <c r="C831" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C212:C253 C441:C484 C408:C439 C333:C406 C324:C331 C305:C322 C263:C303 C255:C261 C715:C831 C486:C501">
+  <conditionalFormatting sqref="C212:C253 C441:C463 C408:C439 C333:C406 C324:C331 C305:C322 C263:C303 C255:C261 C715:C831 C486:C501 C469:C484">
+    <cfRule type="duplicateValues" dxfId="45" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C440">
+    <cfRule type="duplicateValues" dxfId="44" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C407">
     <cfRule type="duplicateValues" dxfId="43" priority="46"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C440">
+  <conditionalFormatting sqref="C332">
     <cfRule type="duplicateValues" dxfId="42" priority="45"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C407">
+  <conditionalFormatting sqref="C323">
     <cfRule type="duplicateValues" dxfId="41" priority="44"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C332">
+  <conditionalFormatting sqref="C304">
     <cfRule type="duplicateValues" dxfId="40" priority="43"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C323">
+  <conditionalFormatting sqref="C262">
     <cfRule type="duplicateValues" dxfId="39" priority="42"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C304">
+  <conditionalFormatting sqref="C254">
     <cfRule type="duplicateValues" dxfId="38" priority="41"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C262">
+  <conditionalFormatting sqref="C193">
     <cfRule type="duplicateValues" dxfId="37" priority="40"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C254">
+  <conditionalFormatting sqref="C184">
     <cfRule type="duplicateValues" dxfId="36" priority="39"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C193">
+  <conditionalFormatting sqref="C159">
     <cfRule type="duplicateValues" dxfId="35" priority="38"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C184">
+  <conditionalFormatting sqref="C152:C153">
     <cfRule type="duplicateValues" dxfId="34" priority="37"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C159">
+  <conditionalFormatting sqref="C151">
     <cfRule type="duplicateValues" dxfId="33" priority="36"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C152:C153">
+  <conditionalFormatting sqref="C149">
     <cfRule type="duplicateValues" dxfId="32" priority="35"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C151">
+  <conditionalFormatting sqref="C94">
     <cfRule type="duplicateValues" dxfId="31" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149">
+  <conditionalFormatting sqref="C85">
     <cfRule type="duplicateValues" dxfId="30" priority="33"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C94">
+  <conditionalFormatting sqref="C63">
     <cfRule type="duplicateValues" dxfId="29" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C48">
     <cfRule type="duplicateValues" dxfId="28" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="duplicateValues" dxfId="27" priority="30"/>
+  <conditionalFormatting sqref="C20 C14:C17 C10:C11 C25 C8 C704:C713 C651:C696 C638:C649 C618:C636 C607:C616 C600:C605 C591:C598 C577:C589 C544:C565 C518:C519 C521:C542 C513 C702">
+    <cfRule type="duplicateValues" dxfId="27" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="duplicateValues" dxfId="26" priority="29"/>
+  <conditionalFormatting sqref="C650">
+    <cfRule type="duplicateValues" dxfId="26" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20 C14:C17 C10:C11 C25 C8 C704:C713 C651:C702 C638:C649 C618:C636 C607:C616 C600:C605 C591:C598 C577:C589 C544:C565 C518:C519 C521:C542 C513">
+  <conditionalFormatting sqref="C637">
     <cfRule type="duplicateValues" dxfId="25" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C650">
+  <conditionalFormatting sqref="C617">
     <cfRule type="duplicateValues" dxfId="24" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C637">
+  <conditionalFormatting sqref="C606">
     <cfRule type="duplicateValues" dxfId="23" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C617">
+  <conditionalFormatting sqref="C599">
     <cfRule type="duplicateValues" dxfId="22" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C606">
+  <conditionalFormatting sqref="C590">
     <cfRule type="duplicateValues" dxfId="21" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C599">
+  <conditionalFormatting sqref="C576">
     <cfRule type="duplicateValues" dxfId="20" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C590">
+  <conditionalFormatting sqref="C572:C575">
     <cfRule type="duplicateValues" dxfId="19" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C576">
+  <conditionalFormatting sqref="C566:C571">
     <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C572:C575">
+  <conditionalFormatting sqref="C543">
     <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C566:C571">
+  <conditionalFormatting sqref="C511">
     <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C543">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  <conditionalFormatting sqref="C7 C5">
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C511">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C5">
+  <conditionalFormatting sqref="C502:C505">
     <cfRule type="duplicateValues" dxfId="13" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
+  <conditionalFormatting sqref="C506:C510">
     <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C502:C505">
+  <conditionalFormatting sqref="C12">
     <cfRule type="duplicateValues" dxfId="11" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C506:C510">
+  <conditionalFormatting sqref="C512">
     <cfRule type="duplicateValues" dxfId="10" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+  <conditionalFormatting sqref="C515:C517">
     <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C512">
+  <conditionalFormatting sqref="C514">
     <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C515:C517">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C514">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C13 C6 C194:C211 C185:C192 C160:C183 C154:C158 C150 C95:C148 C86:C93 C64:C84 C49:C62 C26:C47 C18:C19 C21:C24">
-    <cfRule type="duplicateValues" dxfId="5" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C520">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C485">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C485">
+  <conditionalFormatting sqref="C3">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
+  <conditionalFormatting sqref="C9">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
+  <conditionalFormatting sqref="C464:C468">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+  <conditionalFormatting sqref="C697:C701">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>